<commit_message>
Hello I have lot of files added and modification
</commit_message>
<xml_diff>
--- a/Writesheet.xlsx
+++ b/Writesheet.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="54">
   <si>
     <t>First Name</t>
   </si>
@@ -813,9 +813,6 @@
       <c r="H3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I3" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -841,9 +838,6 @@
       </c>
       <c r="H4" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="I4" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>